<commit_message>
feature | i-491 | campos cotizacion, campo pdf factura (marca)
</commit_message>
<xml_diff>
--- a/public/formats/item_sets.xlsx
+++ b/public/formats/item_sets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BREM\Desktop\zzzzzzzzz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF42DBF-BB45-4D74-B5E2-F967DF367E69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12330"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Código Interno</t>
   </si>
@@ -84,12 +85,39 @@
   </si>
   <si>
     <t>CODKIT2</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Nombre secundario</t>
+  </si>
+  <si>
+    <t>desc 1</t>
+  </si>
+  <si>
+    <t>desc 2</t>
+  </si>
+  <si>
+    <t>nombre sec 1</t>
+  </si>
+  <si>
+    <t>nombre sec 2</t>
+  </si>
+  <si>
+    <t>Plataforma</t>
+  </si>
+  <si>
+    <t>Saga Falabella</t>
+  </si>
+  <si>
+    <t>Linio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,11 +429,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,11 +448,11 @@
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -452,8 +480,17 @@
       <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -481,8 +518,17 @@
       <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -509,10 +555,19 @@
       </c>
       <c r="I3" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan validaciones en form retenciones - validacion codigo respuesta - gestion de cdr
</commit_message>
<xml_diff>
--- a/public/formats/item_sets.xlsx
+++ b/public/formats/item_sets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF42DBF-BB45-4D74-B5E2-F967DF367E69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447C9199-54A4-4AE4-92EA-018586E0B386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Código Interno</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>Linio</t>
+  </si>
+  <si>
+    <t>Tiene Igv</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -147,7 +156,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -430,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +462,7 @@
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -489,8 +499,11 @@
       <c r="L1" t="s">
         <v>26</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -527,8 +540,11 @@
       <c r="L2" t="s">
         <v>27</v>
       </c>
+      <c r="M2" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -564,6 +580,9 @@
       </c>
       <c r="L3" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>